<commit_message>
fab files generated 2 pcbway
</commit_message>
<xml_diff>
--- a/backplane-boards/backplane-breakout-big/backplane-breaout-big.xlsx
+++ b/backplane-boards/backplane-breakout-big/backplane-breaout-big.xlsx
@@ -1,52 +1,207 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caden\Documents\GitHub\backplane\backplane-boards\backplane-rbf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Github\backplane\backplane-boards\backplane-breakout-big\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1E5A57C5-FB55-4EEB-9BA8-79DEA49C2C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24210" windowHeight="10815"/>
   </bookViews>
   <sheets>
-    <sheet name="backplane-rbf" sheetId="1" r:id="rId1"/>
+    <sheet name="backplane-breaout-big" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Footprint</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Manufacturer Part Number 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1 J2 </t>
-  </si>
-  <si>
-    <t>backplane-rbf:SAMTEC_LSH-030-01-X-D-A-TR</t>
-  </si>
-  <si>
-    <t>LSH-030-01-X-D-A-TR</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Reference(s)</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Footprint</t>
+  </si>
+  <si>
+    <t>Manufacturer Part Number 1</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>LED_SMD:LED_0603_1608Metric_Castellated</t>
+  </si>
+  <si>
+    <t>LTST-C191KRKT</t>
+  </si>
+  <si>
+    <t>GREEN</t>
+  </si>
+  <si>
+    <t>LTST-C191KGKT</t>
+  </si>
+  <si>
+    <t>BLUE</t>
+  </si>
+  <si>
+    <t>LTST-C191TBKT</t>
+  </si>
+  <si>
+    <t>ORANGE</t>
+  </si>
+  <si>
+    <t>LTST-C191KFKT</t>
+  </si>
+  <si>
+    <t>Connector_PinHeader_2.54mm:PinHeader_2x26_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>Breakout Connector</t>
+  </si>
+  <si>
+    <t>backplane-breakout-big:SAMTEC_FTSH-130-04-L-DH_flipped</t>
+  </si>
+  <si>
+    <t>FTSH-130-04-L-DH</t>
+  </si>
+  <si>
+    <t>Connector_PinHeader_2.54mm:PinHeader_2x04_P2.54mm_Vertical_SMD</t>
+  </si>
+  <si>
+    <t>SSM-130-L-DV</t>
+  </si>
+  <si>
+    <t>backplane-breakout-big:SAMTEC_SSM-130-L-DV</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>HSEC8-160-01-S-DV-A-K-TR</t>
+  </si>
+  <si>
+    <t>backplane-breakout-big:HSEC8-160-01-S-DV-A-K-TR</t>
+  </si>
+  <si>
+    <t>BSS84W-7-F</t>
+  </si>
+  <si>
+    <t>Package_TO_SOT_SMD:SOT-323_SC-70</t>
+  </si>
+  <si>
+    <t>DMG1012UW-7</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>Resistor_SMD:R_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>BUS_RESET</t>
+  </si>
+  <si>
+    <t>backplane-breakout-big:SW_2-1437565-9</t>
+  </si>
+  <si>
+    <t>2-1437565-9</t>
+  </si>
+  <si>
+    <t>USER_SW_1</t>
+  </si>
+  <si>
+    <t>backplane-breakout-big:JS102011SCQN</t>
+  </si>
+  <si>
+    <t>JS102011SCQN</t>
+  </si>
+  <si>
+    <t>backplane-breakout-big:Keystone_5027</t>
+  </si>
+  <si>
+    <t>Keystone 5027</t>
+  </si>
+  <si>
+    <t>D1, D4, D5, D6, D9, D10, D13</t>
+  </si>
+  <si>
+    <t>D2, D3, D7, D8, D11, D12, D14, D15</t>
+  </si>
+  <si>
+    <t>D16, D19, D22, D23</t>
+  </si>
+  <si>
+    <t>D17, D18, D20, D21</t>
+  </si>
+  <si>
+    <t>H1, H2</t>
+  </si>
+  <si>
+    <t>J4, J5</t>
+  </si>
+  <si>
+    <t>Q1, Q4, Q5, Q6, Q9, Q10, Q13</t>
+  </si>
+  <si>
+    <t>Q2, Q3, Q7, Q8, Q11, Q12, Q14, Q15, Q16, Q17, Q18, Q19, Q20, Q21, Q22, Q23</t>
+  </si>
+  <si>
+    <t>R1, R2, R8, R9, R14, R15, R20, R21, R24, R25, R26, R27, R32, R33, R34, R35</t>
+  </si>
+  <si>
+    <t>R3, R4, R5, R6, R7, R10, R11, R12, R13, R16, R17, R18, R19, R22, R23, R28, R29, R30, R31, R36, R37, R38, R39</t>
+  </si>
+  <si>
+    <t>ESQ-132-12-G-D</t>
+  </si>
+  <si>
+    <t>J1, J2</t>
+  </si>
+  <si>
+    <t>HLE-104-02-G-DV-P-TR</t>
+  </si>
+  <si>
+    <t>J3, J6, J7</t>
+  </si>
+  <si>
+    <t>SW1,  SW2</t>
+  </si>
+  <si>
+    <t>SW3, SW4, SW5, SW6, SW7, SW8, SW9, SW10, SW11</t>
+  </si>
+  <si>
+    <t>PC/104 Headers</t>
+  </si>
+  <si>
+    <t>TP1 thru TP120</t>
+  </si>
+  <si>
+    <t>ESR03EZPF1001</t>
+  </si>
+  <si>
+    <t>RMCF0603FT100K</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -109,7 +264,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C5700"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -502,27 +657,27 @@
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -601,7 +756,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -613,7 +768,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -630,9 +785,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -660,31 +815,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -712,23 +850,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -881,13 +1002,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="93.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="67.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -900,22 +1029,350 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A15" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>A7+1</f>
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>A9+1</f>
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f>A15+1</f>
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f>A16+1</f>
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>120</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minor bom issues corrected
</commit_message>
<xml_diff>
--- a/backplane-boards/backplane-breakout-big/backplane-breaout-big.xlsx
+++ b/backplane-boards/backplane-breakout-big/backplane-breaout-big.xlsx
@@ -1,20 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Github\backplane\backplane-boards\backplane-breakout-big\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caden\Documents\GitHub\backplane\backplane-boards\backplane-breakout-big\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6980040A-AD54-48B2-BBAE-4583EF53E474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24210" windowHeight="10815"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="backplane-breaout-big" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -168,9 +180,6 @@
     <t>R3, R4, R5, R6, R7, R10, R11, R12, R13, R16, R17, R18, R19, R22, R23, R28, R29, R30, R31, R36, R37, R38, R39</t>
   </si>
   <si>
-    <t>ESQ-132-12-G-D</t>
-  </si>
-  <si>
     <t>J1, J2</t>
   </si>
   <si>
@@ -195,13 +204,16 @@
     <t>ESR03EZPF1001</t>
   </si>
   <si>
-    <t>RMCF0603FT100K</t>
+    <t>ESQ-126-12-G-D</t>
+  </si>
+  <si>
+    <t>RMCF0603FT10K0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1001,11 +1013,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,13 +1143,13 @@
         <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
         <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1149,7 +1161,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
@@ -1191,16 +1203,16 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
         <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1305,7 +1317,7 @@
         <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1317,7 +1329,7 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
         <v>31</v>
@@ -1338,7 +1350,7 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D16" t="s">
         <v>34</v>
@@ -1359,7 +1371,7 @@
         <v>120</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" t="s">
         <v>38</v>

</xml_diff>